<commit_message>
Tested stimulated stock. Fixed bug with calculating appreciation
</commit_message>
<xml_diff>
--- a/ExcelExports/Stock 1.xlsx
+++ b/ExcelExports/Stock 1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="31">
   <si>
     <t/>
   </si>
@@ -52,7 +52,7 @@
     <t>asset_value</t>
   </si>
   <si>
-    <t>invested_capital</t>
+    <t>capital_invested</t>
   </si>
   <si>
     <t>effective_income</t>
@@ -103,10 +103,13 @@
     <t>Month: 13</t>
   </si>
   <si>
-    <t>Dividends</t>
-  </si>
-  <si>
-    <t>Capital Appreciation</t>
+    <t>Dividend</t>
+  </si>
+  <si>
+    <t>Dividend Reinvestment</t>
+  </si>
+  <si>
+    <t>Market Growth</t>
   </si>
 </sst>
 </file>
@@ -236,7 +239,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="n" s="0">
         <v>0.0</v>
@@ -251,7 +254,7 @@
         <v>0.0</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.0797414043</v>
       </c>
       <c r="G2" t="n" s="0">
         <v>0.0</v>
@@ -260,24 +263,24 @@
         <v>0.0</v>
       </c>
       <c r="I2" t="n" s="0">
-        <v>11.0</v>
+        <v>10.0797414043</v>
       </c>
       <c r="J2" t="n" s="0">
-        <v>11.0</v>
+        <v>10.0797414043</v>
       </c>
       <c r="K2" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.0797414043</v>
       </c>
       <c r="M2" t="n" s="0">
-        <v>1.8409443766154858</v>
+        <v>0.09917416475042096</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" t="n" s="0">
         <v>0.0</v>
@@ -292,7 +295,7 @@
         <v>0.0</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08101314261194721</v>
       </c>
       <c r="G3" t="n" s="0">
         <v>0.0</v>
@@ -301,24 +304,24 @@
         <v>0.0</v>
       </c>
       <c r="I3" t="n" s="0">
-        <v>12.0</v>
+        <v>10.160754546911948</v>
       </c>
       <c r="J3" t="n" s="0">
-        <v>12.0</v>
+        <v>10.160754546911948</v>
       </c>
       <c r="K3" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L3" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08101314261194721</v>
       </c>
       <c r="M3" t="n" s="0">
-        <v>1.6130352902246758</v>
+        <v>0.09998692994627234</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B4" t="n" s="0">
         <v>0.0</v>
@@ -333,7 +336,7 @@
         <v>0.0</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>1.0</v>
+        <v>0.0823051629636738</v>
       </c>
       <c r="G4" t="n" s="0">
         <v>0.0</v>
@@ -342,24 +345,24 @@
         <v>0.0</v>
       </c>
       <c r="I4" t="n" s="0">
-        <v>13.0</v>
+        <v>10.243059709875622</v>
       </c>
       <c r="J4" t="n" s="0">
-        <v>13.0</v>
+        <v>10.243059709875622</v>
       </c>
       <c r="K4" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L4" t="n" s="0">
-        <v>1.0</v>
+        <v>0.0823051629636738</v>
       </c>
       <c r="M4" t="n" s="0">
-        <v>1.4334151101796073</v>
+        <v>0.10080004237548734</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n" s="0">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B5" t="n" s="0">
         <v>0.0</v>
@@ -374,7 +377,7 @@
         <v>0.0</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08361778881884652</v>
       </c>
       <c r="G5" t="n" s="0">
         <v>0.0</v>
@@ -383,24 +386,24 @@
         <v>0.0</v>
       </c>
       <c r="I5" t="n" s="0">
-        <v>14.0</v>
+        <v>10.326677498694469</v>
       </c>
       <c r="J5" t="n" s="0">
-        <v>14.0</v>
+        <v>10.326677498694469</v>
       </c>
       <c r="K5" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L5" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08361778881884652</v>
       </c>
       <c r="M5" t="n" s="0">
-        <v>1.2885409112665345</v>
+        <v>0.10161340020425058</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n" s="0">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="B6" t="n" s="0">
         <v>0.0</v>
@@ -415,7 +418,7 @@
         <v>0.0</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08495134879982165</v>
       </c>
       <c r="G6" t="n" s="0">
         <v>0.0</v>
@@ -424,24 +427,24 @@
         <v>0.0</v>
       </c>
       <c r="I6" t="n" s="0">
-        <v>15.0</v>
+        <v>10.41162884749429</v>
       </c>
       <c r="J6" t="n" s="0">
-        <v>15.0</v>
+        <v>10.41162884749429</v>
       </c>
       <c r="K6" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L6" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08495134879982165</v>
       </c>
       <c r="M6" t="n" s="0">
-        <v>1.1694252129716127</v>
+        <v>0.10242690147587585</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n" s="0">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="B7" t="n" s="0">
         <v>0.0</v>
@@ -456,7 +459,7 @@
         <v>0.0</v>
       </c>
       <c r="F7" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08630617676991702</v>
       </c>
       <c r="G7" t="n" s="0">
         <v>0.0</v>
@@ -465,24 +468,24 @@
         <v>0.0</v>
       </c>
       <c r="I7" t="n" s="0">
-        <v>16.0</v>
+        <v>10.497935024264207</v>
       </c>
       <c r="J7" t="n" s="0">
-        <v>16.0</v>
+        <v>10.497935024264207</v>
       </c>
       <c r="K7" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L7" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08630617676991702</v>
       </c>
       <c r="M7" t="n" s="0">
-        <v>1.0698899917795224</v>
+        <v>0.10324044416197853</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n" s="0">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="B8" t="n" s="0">
         <v>0.0</v>
@@ -497,7 +500,7 @@
         <v>0.0</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08768261191699647</v>
       </c>
       <c r="G8" t="n" s="0">
         <v>0.0</v>
@@ -506,24 +509,24 @@
         <v>0.0</v>
       </c>
       <c r="I8" t="n" s="0">
-        <v>17.0</v>
+        <v>10.585617636181203</v>
       </c>
       <c r="J8" t="n" s="0">
-        <v>17.0</v>
+        <v>10.585617636181203</v>
       </c>
       <c r="K8" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L8" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08768261191699647</v>
       </c>
       <c r="M8" t="n" s="0">
-        <v>0.9855599520654272</v>
+        <v>0.10405392621369414</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n" s="0">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="B9" t="n" s="0">
         <v>0.0</v>
@@ -538,7 +541,7 @@
         <v>0.0</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>1.0</v>
+        <v>0.0890809988383871</v>
       </c>
       <c r="G9" t="n" s="0">
         <v>0.0</v>
@@ -547,24 +550,24 @@
         <v>0.0</v>
       </c>
       <c r="I9" t="n" s="0">
-        <v>18.0</v>
+        <v>10.67469863501959</v>
       </c>
       <c r="J9" t="n" s="0">
-        <v>18.0</v>
+        <v>10.67469863501959</v>
       </c>
       <c r="K9" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L9" t="n" s="0">
-        <v>1.0</v>
+        <v>0.0890809988383871</v>
       </c>
       <c r="M9" t="n" s="0">
-        <v>0.9132562918007303</v>
+        <v>0.10486724561293181</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n" s="0">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="B10" t="n" s="0">
         <v>0.0</v>
@@ -579,7 +582,7 @@
         <v>0.0</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09050168762715104</v>
       </c>
       <c r="G10" t="n" s="0">
         <v>0.0</v>
@@ -588,24 +591,24 @@
         <v>0.0</v>
       </c>
       <c r="I10" t="n" s="0">
-        <v>19.0</v>
+        <v>10.765200322646741</v>
       </c>
       <c r="J10" t="n" s="0">
-        <v>19.0</v>
+        <v>10.765200322646741</v>
       </c>
       <c r="K10" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L10" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09050168762715104</v>
       </c>
       <c r="M10" t="n" s="0">
-        <v>0.8506178062217085</v>
+        <v>0.10568030042360554</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n" s="0">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="B11" t="n" s="0">
         <v>0.0</v>
@@ -620,7 +623,7 @@
         <v>0.0</v>
       </c>
       <c r="F11" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09194503395973284</v>
       </c>
       <c r="G11" t="n" s="0">
         <v>0.0</v>
@@ -629,24 +632,24 @@
         <v>0.0</v>
       </c>
       <c r="I11" t="n" s="0">
-        <v>20.0</v>
+        <v>10.857145356606475</v>
       </c>
       <c r="J11" t="n" s="0">
-        <v>20.0</v>
+        <v>10.857145356606475</v>
       </c>
       <c r="K11" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L11" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09194503395973284</v>
       </c>
       <c r="M11" t="n" s="0">
-        <v>0.7958563260221301</v>
+        <v>0.10649298884274239</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n" s="0">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="B12" t="n" s="0">
         <v>0.0</v>
@@ -661,7 +664,7 @@
         <v>0.0</v>
       </c>
       <c r="F12" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09341139918500489</v>
       </c>
       <c r="G12" t="n" s="0">
         <v>0.0</v>
@@ -670,24 +673,24 @@
         <v>0.0</v>
       </c>
       <c r="I12" t="n" s="0">
-        <v>21.0</v>
+        <v>10.95055675579148</v>
       </c>
       <c r="J12" t="n" s="0">
-        <v>21.0</v>
+        <v>10.95055675579148</v>
       </c>
       <c r="K12" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L12" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09341139918500489</v>
       </c>
       <c r="M12" t="n" s="0">
-        <v>0.7475943544285117</v>
+        <v>0.10730520925149789</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n" s="0">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="B13" t="n" s="0">
         <v>0.0</v>
@@ -702,7 +705,7 @@
         <v>0.0</v>
       </c>
       <c r="F13" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09490115041473293</v>
       </c>
       <c r="G13" t="n" s="0">
         <v>0.0</v>
@@ -711,24 +714,24 @@
         <v>0.0</v>
       </c>
       <c r="I13" t="n" s="0">
-        <v>22.0</v>
+        <v>11.045457906206213</v>
       </c>
       <c r="J13" t="n" s="0">
-        <v>22.0</v>
+        <v>11.045457906206213</v>
       </c>
       <c r="K13" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L13" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09490115041473293</v>
       </c>
       <c r="M13" t="n" s="0">
-        <v>0.7047545660620107</v>
+        <v>0.10811686026592171</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n" s="0">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="B14" t="n" s="0">
         <v>0.0</v>
@@ -743,7 +746,7 @@
         <v>0.0</v>
       </c>
       <c r="F14" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09641466061548419</v>
       </c>
       <c r="G14" t="n" s="0">
         <v>0.0</v>
@@ -752,24 +755,24 @@
         <v>0.0</v>
       </c>
       <c r="I14" t="n" s="0">
-        <v>23.0</v>
+        <v>11.141872566821696</v>
       </c>
       <c r="J14" t="n" s="0">
-        <v>23.0</v>
+        <v>11.141872566821696</v>
       </c>
       <c r="K14" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L14" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09641466061548419</v>
       </c>
       <c r="M14" t="n" s="0">
-        <v>0.6664829255615827</v>
+        <v>0.1089278407875176</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n" s="0">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="B15" t="n" s="0">
         <v>0.0</v>
@@ -784,7 +787,7 @@
         <v>0.0</v>
       </c>
       <c r="F15" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09795230870200153</v>
       </c>
       <c r="G15" t="n" s="0">
         <v>0.0</v>
@@ -793,19 +796,19 @@
         <v>0.0</v>
       </c>
       <c r="I15" t="n" s="0">
-        <v>24.0</v>
+        <v>11.239824875523698</v>
       </c>
       <c r="J15" t="n" s="0">
-        <v>24.0</v>
+        <v>11.239824875523698</v>
       </c>
       <c r="K15" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L15" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09795230870200153</v>
       </c>
       <c r="M15" t="n" s="0">
-        <v>0.6320941327229255</v>
+        <v>0.10973805005346815</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +818,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN2"/>
+  <dimension ref="A1:AO2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -866,28 +869,88 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>0.0</v>
+      </c>
       <c r="G2" t="s" s="0">
         <v>28</v>
       </c>
       <c r="H2" t="n" s="0">
         <v>0.0</v>
       </c>
+      <c r="J2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="K2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="N2" t="n" s="0">
+        <v>0.0</v>
+      </c>
       <c r="P2" t="s" s="0">
         <v>28</v>
       </c>
       <c r="Q2" t="n" s="0">
         <v>0.0</v>
       </c>
+      <c r="S2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="T2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="W2" t="n" s="0">
+        <v>0.0</v>
+      </c>
       <c r="Y2" t="s" s="0">
         <v>28</v>
       </c>
       <c r="Z2" t="n" s="0">
         <v>0.0</v>
       </c>
+      <c r="AB2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="AC2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AE2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="AF2" t="n" s="0">
+        <v>0.0</v>
+      </c>
       <c r="AH2" t="s" s="0">
         <v>28</v>
       </c>
       <c r="AI2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AK2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="AL2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AN2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="AO2" t="n" s="0">
         <v>0.0</v>
       </c>
     </row>
@@ -1012,7 +1075,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN1"/>
+  <dimension ref="A1:AO2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1060,6 +1123,92 @@
       </c>
       <c r="AN1" t="s" s="5">
         <v>27</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="K2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="N2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="T2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="W2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="Z2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="AC2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AE2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="AF2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AH2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="AI2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AK2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="AL2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AN2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="AO2" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -1121,88 +1270,88 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.0797414043</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08101314261194721</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.0823051629636738</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08361778881884652</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08495134879982165</v>
       </c>
       <c r="P2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08630617676991702</v>
       </c>
       <c r="S2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="T2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.08768261191699647</v>
       </c>
       <c r="V2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="W2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.0890809988383871</v>
       </c>
       <c r="Y2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Z2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09050168762715104</v>
       </c>
       <c r="AB2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09194503395973284</v>
       </c>
       <c r="AE2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AF2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09341139918500489</v>
       </c>
       <c r="AH2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AI2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09490115041473293</v>
       </c>
       <c r="AK2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AL2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09641466061548419</v>
       </c>
       <c r="AN2" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AO2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.09795230870200153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>